<commit_message>
Created minimal BFO to IES mapping by adding some structure to the IES event class.
</commit_message>
<xml_diff>
--- a/projects/project-3/assignment/src/data/bfo-core-ies-structural-matches-with-defs.xlsx
+++ b/projects/project-3/assignment/src/data/bfo-core-ies-structural-matches-with-defs.xlsx
@@ -488,29 +488,52 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/BFO_0000027</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>http://purl.obolibrary.org/obo/BFO_0000015</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>R:only×3</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>SubClassOf: ns1:BFO_0000003 | SubClassOf: ns1:BFO_0000117 only (ns1:BFO_0000015 OR ns1:BFO_0000035) | SubClassOf: ns1:BFO_0000132 only ns1:BFO_0000015 | SubClassOf: ns1:BFO_0000139 only ns1:BFO_0000015</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://ies.data.gov.uk/ontology/ies4#DispositionalClass</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t>http://ies.data.gov.uk/ontology/ies4#Event</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>R:only</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>SubClassOf: ies:Element | SubClassOf: ns1:BFO_0000015 | SubClassOf: ns1:BFO_0000178 only (ns1:BFO_0000029 OR ns1:BFO_0000140)</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(Elucidation) An object aggregate is a material entity consisting exactly of a plurality (≥1) of objects as member parts which together form a unit</t>
+          <t>(Elucidation) p is a process means p is an occurrent that has some temporal proper part and for some time t, p has some material entity as participant</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>A ClassOfElement whose instances all share the same disposition - e.g. capability or tendency
-Example: Vehicles capable of Mach 2</t>
+          <t>An Event represents an activity or incident, involving one or more participating entities, that occurred/started at a specific point in time – e.g. a meeting, or a telephone call.</t>
         </is>
       </c>
     </row>

</xml_diff>